<commit_message>
Uploaded revised info template
</commit_message>
<xml_diff>
--- a/Information Template V2.xlsx
+++ b/Information Template V2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Floor Area 
 (m2)</t>
@@ -33,30 +33,18 @@
     <t>Address</t>
   </si>
   <si>
-    <t xml:space="preserve">Passing Rent </t>
-  </si>
-  <si>
-    <t>Gross/Net/Semi-Gross</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rent Incentives </t>
   </si>
   <si>
     <t>Other details (if any)</t>
   </si>
   <si>
-    <t>Property Type</t>
-  </si>
-  <si>
     <t>Level in Building</t>
   </si>
   <si>
     <t>Agency</t>
   </si>
   <si>
-    <t>Agent</t>
-  </si>
-  <si>
     <t>Municipality</t>
   </si>
   <si>
@@ -76,6 +64,17 @@
   </si>
   <si>
     <t xml:space="preserve">Tenant Trading Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passing Rent/
+Asking Rent </t>
+  </si>
+  <si>
+    <t>Primary Use</t>
+  </si>
+  <si>
+    <t>Gross/Net/
+Semi-Gross</t>
   </si>
 </sst>
 </file>
@@ -212,7 +211,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -280,6 +279,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -342,7 +342,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1495423</xdr:colOff>
+      <xdr:colOff>1819273</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1422442</xdr:rowOff>
     </xdr:to>
@@ -657,22 +657,22 @@
   <dimension ref="B1:V50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="9" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="18" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="18" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" customWidth="1"/>
     <col min="15" max="15" width="27.28515625" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
@@ -684,7 +684,7 @@
     </row>
     <row r="2" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -702,9 +702,7 @@
       <c r="P2" s="27"/>
     </row>
     <row r="3" spans="2:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>9</v>
-      </c>
+      <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
@@ -728,49 +726,49 @@
     </row>
     <row r="4" spans="2:22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="O4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="24" t="s">
         <v>3</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="24" t="s">
-        <v>5</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -788,9 +786,9 @@
       <c r="G5" s="11"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="11"/>
+      <c r="J5" s="19"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="L5" s="29"/>
       <c r="M5" s="19"/>
       <c r="N5" s="13"/>
       <c r="O5" s="11"/>

</xml_diff>

<commit_message>
Fixed formatting off template and deployed app
</commit_message>
<xml_diff>
--- a/Information Template V2.xlsx
+++ b/Information Template V2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Newer Docs\Databases\Mailout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Personal\mailout\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD39F15-8168-419F-8C1D-365303146457}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="City Council Questionnaire" sheetId="1" r:id="rId1"/>
@@ -80,10 +81,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -204,14 +207,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -232,32 +236,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -273,17 +253,90 @@
     <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Comma" xfId="5" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="3"/>
+    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
@@ -348,7 +401,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Westlink Consulting Team Site"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Westlink Consulting Team Site">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -653,26 +712,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="8" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="8" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="9" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" customWidth="1"/>
     <col min="15" max="15" width="27.28515625" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
@@ -683,40 +742,40 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="2:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -725,49 +784,49 @@
       <c r="V3" s="5"/>
     </row>
     <row r="4" spans="2:22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="Q4" s="3"/>
@@ -777,152 +836,806 @@
       <c r="U4" s="2"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="2:22" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-    </row>
-    <row r="6" spans="2:22" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-    </row>
-    <row r="7" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M7" s="18"/>
-    </row>
-    <row r="8" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M8" s="18"/>
-    </row>
-    <row r="9" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M9" s="18"/>
-    </row>
-    <row r="10" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="21"/>
-      <c r="M10" s="18"/>
-    </row>
-    <row r="11" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="21"/>
-      <c r="M11" s="18"/>
-    </row>
-    <row r="12" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M12" s="18"/>
-    </row>
-    <row r="13" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M13" s="18"/>
-    </row>
-    <row r="14" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M14" s="18"/>
-    </row>
-    <row r="15" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M15" s="18"/>
-    </row>
-    <row r="16" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M16" s="18"/>
-    </row>
-    <row r="17" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M17" s="18"/>
-    </row>
-    <row r="18" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M18" s="18"/>
-    </row>
-    <row r="19" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M19" s="18"/>
-    </row>
-    <row r="20" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M20" s="18"/>
-    </row>
-    <row r="21" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M21" s="18"/>
-    </row>
-    <row r="22" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M22" s="18"/>
-    </row>
-    <row r="23" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M23" s="18"/>
-    </row>
-    <row r="24" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M24" s="18"/>
-    </row>
-    <row r="25" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M25" s="18"/>
-    </row>
-    <row r="26" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M26" s="18"/>
-    </row>
-    <row r="27" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M27" s="18"/>
-    </row>
-    <row r="28" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M28" s="18"/>
-    </row>
-    <row r="29" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M29" s="18"/>
-    </row>
-    <row r="30" spans="13:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M30" s="18"/>
-    </row>
-    <row r="31" spans="13:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="13:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:22" s="20" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+    </row>
+    <row r="6" spans="2:22" s="20" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+    </row>
+    <row r="7" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+    </row>
+    <row r="8" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+    </row>
+    <row r="9" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+    </row>
+    <row r="10" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+    </row>
+    <row r="11" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+    </row>
+    <row r="12" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+    </row>
+    <row r="13" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+    </row>
+    <row r="14" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+    </row>
+    <row r="15" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+    </row>
+    <row r="16" spans="2:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+    </row>
+    <row r="17" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+    </row>
+    <row r="18" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+    </row>
+    <row r="19" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+    </row>
+    <row r="20" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+    </row>
+    <row r="21" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+    </row>
+    <row r="22" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+    </row>
+    <row r="23" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+    </row>
+    <row r="24" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+    </row>
+    <row r="25" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+    </row>
+    <row r="26" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="41"/>
+      <c r="P40" s="41"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+      <c r="O41" s="41"/>
+      <c r="P41" s="41"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="41"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="41"/>
+      <c r="O43" s="41"/>
+      <c r="P43" s="41"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="41"/>
+      <c r="P44" s="41"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="41"/>
+      <c r="P45" s="41"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="41"/>
+      <c r="P46" s="41"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="41"/>
+      <c r="P47" s="41"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="41"/>
+      <c r="O48" s="41"/>
+      <c r="P48" s="41"/>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="40"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="41"/>
+      <c r="O49" s="41"/>
+      <c r="P49" s="41"/>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="41"/>
+      <c r="O50" s="41"/>
+      <c r="P50" s="41"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:P50">
+  <conditionalFormatting sqref="B7:P26">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(ISBLANK($C7))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added new info template
</commit_message>
<xml_diff>
--- a/Information Template V2.xlsx
+++ b/Information Template V2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Floor Area 
 (m2)</t>
@@ -39,9 +39,6 @@
     <t>Other details (if any)</t>
   </si>
   <si>
-    <t>Level in Building</t>
-  </si>
-  <si>
     <t>Agency</t>
   </si>
   <si>
@@ -75,16 +72,26 @@
   <si>
     <t>Gross/Net/
 Semi-Gross</t>
+  </si>
+  <si>
+    <t>Agent Name</t>
+  </si>
+  <si>
+    <t>Estimated Outgoings</t>
+  </si>
+  <si>
+    <t>Est. Outgoings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -212,7 +219,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -265,7 +272,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -305,6 +311,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -679,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V50"/>
+  <dimension ref="B1:W50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,527 +700,561 @@
     <col min="2" max="2" width="18.7109375" style="9" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="9" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="12" width="12.7109375" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" style="11" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" customWidth="1"/>
     <col min="15" max="15" width="27.28515625" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="D1"/>
     </row>
-    <row r="2" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-    </row>
-    <row r="3" spans="2:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="7"/>
+    <row r="2" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+    </row>
+    <row r="3" spans="2:23" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
-      <c r="T3" s="6"/>
+      <c r="T3" s="7"/>
       <c r="U3" s="6"/>
-      <c r="V3" s="5"/>
-    </row>
-    <row r="4" spans="2:22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="6"/>
+      <c r="W3" s="5"/>
+    </row>
+    <row r="4" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>13</v>
-      </c>
       <c r="I4" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="L4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="M4" s="18" t="s">
         <v>9</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>10</v>
       </c>
       <c r="N4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="2"/>
+      <c r="T4" s="3"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="2:22" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="2"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="2:23" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="12"/>
       <c r="D5" s="19"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="7"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-      <c r="T5" s="6"/>
+      <c r="T5" s="7"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
-    </row>
-    <row r="6" spans="2:22" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6" spans="2:23" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="12"/>
       <c r="D6" s="19"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="7"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="6"/>
+      <c r="T6" s="7"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
-    </row>
-    <row r="7" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="20"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-    </row>
-    <row r="8" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="33"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+    </row>
+    <row r="8" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="20"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-    </row>
-    <row r="9" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="33"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+    </row>
+    <row r="9" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="20"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-    </row>
-    <row r="10" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="33"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+    </row>
+    <row r="10" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="13"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-    </row>
-    <row r="11" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="33"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+    </row>
+    <row r="11" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="13"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-    </row>
-    <row r="12" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="33"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+    </row>
+    <row r="12" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="20"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-    </row>
-    <row r="13" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="33"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+    </row>
+    <row r="13" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="20"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-    </row>
-    <row r="14" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="33"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+    </row>
+    <row r="14" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="20"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-    </row>
-    <row r="15" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="33"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+    </row>
+    <row r="15" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-    </row>
-    <row r="16" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="33"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+    </row>
+    <row r="16" spans="2:23" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="20"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-    </row>
-    <row r="17" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="33"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+    </row>
+    <row r="17" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="20"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-    </row>
-    <row r="18" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="33"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+    </row>
+    <row r="18" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="20"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-    </row>
-    <row r="19" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="33"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+    </row>
+    <row r="19" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="20"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-    </row>
-    <row r="20" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="33"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+    </row>
+    <row r="20" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="20"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-    </row>
-    <row r="21" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="33"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+    </row>
+    <row r="21" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="20"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-    </row>
-    <row r="22" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="33"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+    </row>
+    <row r="22" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="20"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-    </row>
-    <row r="23" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="33"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+    </row>
+    <row r="23" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="20"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-    </row>
-    <row r="24" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="33"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+    </row>
+    <row r="24" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="20"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-    </row>
-    <row r="25" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="33"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+    </row>
+    <row r="25" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="20"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-    </row>
-    <row r="26" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="33"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+    </row>
+    <row r="26" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="20"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-    </row>
-    <row r="27" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="33"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+    </row>
+    <row r="27" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="20"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-    </row>
-    <row r="28" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="33"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+    </row>
+    <row r="28" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="20"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-    </row>
-    <row r="29" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="33"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+    </row>
+    <row r="29" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="20"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-    </row>
-    <row r="30" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="33"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+    </row>
+    <row r="30" spans="4:17" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="20"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="26"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-    </row>
-    <row r="31" spans="4:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="4:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="25"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+    </row>
+    <row r="31" spans="4:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="4:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1231,10 +1275,10 @@
     <row r="50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:P50">
+  <conditionalFormatting sqref="B7:Q50">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(ISBLANK($C7))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed app crash and updated template
</commit_message>
<xml_diff>
--- a/Information Template V2.xlsx
+++ b/Information Template V2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Floor Area 
 (m2)</t>
@@ -39,9 +39,6 @@
     <t>Other details (if any)</t>
   </si>
   <si>
-    <t>Level in Building</t>
-  </si>
-  <si>
     <t>Agency</t>
   </si>
   <si>
@@ -75,16 +72,23 @@
   <si>
     <t>Gross/Net/
 Semi-Gross</t>
+  </si>
+  <si>
+    <t>Agent Name</t>
+  </si>
+  <si>
+    <t>Est. Outgoings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -212,7 +216,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -265,7 +269,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -299,6 +302,10 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -682,7 +689,7 @@
   <dimension ref="B1:V50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,11 +697,11 @@
     <col min="2" max="2" width="18.7109375" style="9" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="9" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="12" width="12.7109375" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" style="11" customWidth="1"/>
@@ -708,40 +715,42 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
+      <c r="B2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="2:22" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
+      <c r="B3" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -751,46 +760,46 @@
     </row>
     <row r="4" spans="2:22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>13</v>
-      </c>
       <c r="I4" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="L4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="M4" s="18" t="s">
         <v>9</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>10</v>
       </c>
       <c r="N4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P4" s="16" t="s">
         <v>3</v>
@@ -807,17 +816,17 @@
       <c r="C5" s="12"/>
       <c r="D5" s="19"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
@@ -830,17 +839,17 @@
       <c r="C6" s="12"/>
       <c r="D6" s="19"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -850,364 +859,364 @@
     </row>
     <row r="7" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="20"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
     </row>
     <row r="8" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="20"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
     </row>
     <row r="9" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="20"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="13"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
     </row>
     <row r="11" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="13"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
     </row>
     <row r="12" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="20"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="20"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
     </row>
     <row r="14" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="20"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
     </row>
     <row r="15" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
     </row>
     <row r="16" spans="2:22" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="20"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="20"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="20"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="20"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
     </row>
     <row r="20" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="20"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
     </row>
     <row r="21" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="20"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
     </row>
     <row r="22" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="20"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
     </row>
     <row r="23" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="20"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
     </row>
     <row r="24" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="20"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="20"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
     </row>
     <row r="26" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="20"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
     </row>
     <row r="27" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="20"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
     </row>
     <row r="28" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="20"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
     </row>
     <row r="29" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="20"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
     </row>
     <row r="30" spans="4:16" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="20"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="26"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="25"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
     </row>
     <row r="31" spans="4:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="4:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>